<commit_message>
Updated presentation times in Opioid_Support; added doc tracking my edits to the website
</commit_message>
<xml_diff>
--- a/SupportingMaterial/Opioid_Support.xlsx
+++ b/SupportingMaterial/Opioid_Support.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camke\OneDrive\Education\Berkeley\W210_Capstone\Project\OpiGit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camke\OneDrive\Education\Berkeley\W210_Capstone\Project\OpiGit\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="11_F25DC773A252ABDACC1048B4211D4B9E5ADE58E8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{038975B3-C2F2-425F-8E3D-3ABA8AFCAE92}"/>
+  <xr:revisionPtr revIDLastSave="623" documentId="11_F25DC773A252ABDACC1048B4211D4B9E5ADE58E8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2BDFC200-17EC-43E6-9689-E9A359BFCA00}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="15360" windowHeight="17304" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Comparison" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
   <si>
     <t>Model</t>
   </si>
@@ -129,11 +129,6 @@
   </si>
   <si>
     <t>Wed.
-Dry 
-Run #1</t>
-  </si>
-  <si>
-    <t>Wed.
 In Class</t>
   </si>
   <si>
@@ -483,6 +478,28 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Tues.
+Dry 
+Run</t>
+  </si>
+  <si>
+    <t>Need to reference the mission throughout</t>
+  </si>
+  <si>
+    <t>Wed.
+Dry 
+Run</t>
+  </si>
+  <si>
+    <t>Speed up!</t>
   </si>
 </sst>
 </file>
@@ -490,7 +507,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -526,7 +543,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -534,30 +551,176 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3680,10 +3843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A51846-7BEA-4E25-AD95-1A0EDC9F577F}">
-  <dimension ref="B1:I21"/>
+  <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3691,239 +3854,293 @@
     <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" customWidth="1"/>
-    <col min="5" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.5546875" customWidth="1"/>
+    <col min="5" max="8" width="7.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="11" width="7.5546875" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="2:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G3" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="M3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E4" s="14">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="F4" s="15">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="G4" s="13">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="M4" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="6" t="s">
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="F5" s="15">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="G5" s="13">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.12430555555555556</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.13125000000000001</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" t="s">
+        <v>149</v>
+      </c>
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="13">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="E7" s="14">
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="F7" s="15">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.17430555555555557</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.15694444444444444</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.17916666666666667</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="M8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>6.3194444444444442E-2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>6.7361111111111108E-2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3">
-        <v>4.5138888888888888E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>4.9305555555555554E-2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>5.0694444444444452E-2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.15972222222222224</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.12430555555555556</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5.0694444444444452E-2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>6.8749999999999992E-2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>8.1944444444444445E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D9" s="22">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="E9" s="23">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F9" s="24">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G9" s="22">
+        <v>7.5694444444444439E-2</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="16">
+        <f>SUM(D4:D9)</f>
+        <v>0.57847222222222217</v>
+      </c>
+      <c r="E10" s="17">
+        <f>SUM(E4:E9)</f>
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="F10" s="18">
+        <f>SUM(F4:F9)</f>
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="G10" s="16">
+        <f>SUM(G4:G9)</f>
+        <v>0.58472222222222214</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>147</v>
+      </c>
+      <c r="M12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3">
-        <v>0.17430555555555557</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.15694444444444444</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6.5277777777777782E-2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4">
-        <f>SUM(D3:D8)</f>
-        <v>0.57847222222222217</v>
-      </c>
-      <c r="E9" s="4">
-        <f>SUM(E3:E8)</f>
-        <v>0.53819444444444442</v>
-      </c>
-      <c r="F9" s="4">
-        <f>SUM(F3:F8)</f>
-        <v>0.56597222222222221</v>
-      </c>
-      <c r="I9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I15" t="s">
+      <c r="M17" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H16" t="s">
+    <row r="18" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
+    <row r="19" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="1" t="s">
+    <row r="20" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I19" t="s">
+    <row r="21" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="M21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I20" t="s">
+    <row r="22" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="M22" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I21" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3947,522 +4164,522 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H7" s="7"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H8" s="7"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" s="7"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H10" s="7"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H11" s="7"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H12" s="7"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I13" s="7">
+        <v>113</v>
+      </c>
+      <c r="I13" s="4">
         <v>0.1804</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14">
         <v>68</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="7">
+        <v>86</v>
+      </c>
+      <c r="I14" s="4">
         <v>-5.5899999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
         <v>59</v>
       </c>
-      <c r="G15" t="s">
-        <v>60</v>
-      </c>
       <c r="H15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" s="7">
+        <v>87</v>
+      </c>
+      <c r="I15" s="4">
         <v>-2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
         <v>61</v>
       </c>
-      <c r="G16" t="s">
-        <v>62</v>
-      </c>
       <c r="H16" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="7">
+        <v>88</v>
+      </c>
+      <c r="I16" s="4">
         <v>-7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
         <v>63</v>
       </c>
-      <c r="G17" t="s">
-        <v>64</v>
-      </c>
       <c r="H17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I17" s="7">
+        <v>116</v>
+      </c>
+      <c r="I17" s="4">
         <v>-1.2199999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
         <v>65</v>
       </c>
-      <c r="G18" t="s">
-        <v>66</v>
-      </c>
       <c r="H18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="7">
+        <v>90</v>
+      </c>
+      <c r="I18" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" t="s">
         <v>67</v>
       </c>
-      <c r="G19" t="s">
-        <v>68</v>
-      </c>
       <c r="H19" t="s">
-        <v>92</v>
-      </c>
-      <c r="I19" s="7">
+        <v>91</v>
+      </c>
+      <c r="I19" s="4">
         <v>9.1999999999999998E-3</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
         <v>69</v>
       </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
       <c r="H20" t="s">
-        <v>93</v>
-      </c>
-      <c r="I20" s="7">
+        <v>92</v>
+      </c>
+      <c r="I20" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
-        <v>119</v>
-      </c>
-      <c r="I21" s="7">
+        <v>118</v>
+      </c>
+      <c r="I21" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" s="7">
+        <v>117</v>
+      </c>
+      <c r="I22" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
-      </c>
-      <c r="I23" s="7">
+        <v>95</v>
+      </c>
+      <c r="I23" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
         <v>51</v>
       </c>
-      <c r="G24" t="s">
-        <v>52</v>
-      </c>
       <c r="H24" t="s">
-        <v>116</v>
-      </c>
-      <c r="I24" s="7">
+        <v>115</v>
+      </c>
+      <c r="I24" s="4">
         <v>-1E-3</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
         <v>53</v>
       </c>
-      <c r="G25" t="s">
-        <v>54</v>
-      </c>
       <c r="H25" t="s">
-        <v>120</v>
-      </c>
-      <c r="I25" s="7">
+        <v>119</v>
+      </c>
+      <c r="I25" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H26" t="s">
-        <v>121</v>
-      </c>
-      <c r="I26" s="7">
+        <v>120</v>
+      </c>
+      <c r="I26" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>122</v>
-      </c>
-      <c r="I27" s="7">
+        <v>121</v>
+      </c>
+      <c r="I27" s="4">
         <v>-3.0999999999999999E-3</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" t="s">
-        <v>123</v>
-      </c>
-      <c r="I28" s="7">
+        <v>122</v>
+      </c>
+      <c r="I28" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
-        <v>124</v>
-      </c>
-      <c r="I29" s="7">
+        <v>123</v>
+      </c>
+      <c r="I29" s="4">
         <v>-1.67E-2</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>103</v>
-      </c>
-      <c r="I30" s="7">
+        <v>102</v>
+      </c>
+      <c r="I30" s="4">
         <v>-5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I31" s="7">
+        <v>103</v>
+      </c>
+      <c r="I31" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>105</v>
-      </c>
-      <c r="I32" s="7">
+        <v>104</v>
+      </c>
+      <c r="I32" s="4">
         <v>-1.6999999999999999E-3</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
-      </c>
-      <c r="I33" s="7">
+        <v>124</v>
+      </c>
+      <c r="I33" s="4">
         <v>-7.3000000000000001E-3</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H34" t="s">
-        <v>107</v>
-      </c>
-      <c r="I34" s="7">
+        <v>106</v>
+      </c>
+      <c r="I34" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" s="7">
+        <v>107</v>
+      </c>
+      <c r="I35" s="4">
         <v>-2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H36" t="s">
-        <v>109</v>
-      </c>
-      <c r="I36" s="7">
+        <v>108</v>
+      </c>
+      <c r="I36" s="4">
         <v>-1.8E-3</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H37" t="s">
-        <v>110</v>
-      </c>
-      <c r="I37" s="7">
+        <v>109</v>
+      </c>
+      <c r="I37" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s">
-        <v>126</v>
-      </c>
-      <c r="I38" s="7">
+        <v>125</v>
+      </c>
+      <c r="I38" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s">
-        <v>127</v>
-      </c>
-      <c r="I39" s="7">
+        <v>126</v>
+      </c>
+      <c r="I39" s="4">
         <v>-8.0999999999999996E-3</v>
       </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H40" t="s">
-        <v>128</v>
-      </c>
-      <c r="I40" s="7">
+        <v>127</v>
+      </c>
+      <c r="I40" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H41" t="s">
-        <v>115</v>
-      </c>
-      <c r="I41" s="7">
+        <v>114</v>
+      </c>
+      <c r="I41" s="4">
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H46" s="7">
+      <c r="H46" s="4">
         <f>SUM(I14:I40)</f>
         <v>-0.11639999999999999</v>
       </c>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H48" s="7">
+      <c r="H48" s="4">
         <f>I41-H46</f>
         <v>0.1804</v>
       </c>
@@ -4476,10 +4693,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5DCC5B-780D-4CEA-B28E-7DB62F46FCAC}">
-  <dimension ref="D4:K15"/>
+  <dimension ref="D2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4492,30 +4709,43 @@
     <col min="16" max="16" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="F2" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
     <row r="4" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="G4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="I4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" s="2" t="s">
         <v>137</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.3">
@@ -4525,26 +4755,29 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="6">
+        <f>F$2</f>
         <v>0.2</v>
       </c>
       <c r="G5">
-        <f>($E5-F5)^2</f>
+        <f t="shared" ref="G5:G14" si="0">($E5-F5)^2</f>
         <v>0.64000000000000012</v>
       </c>
-      <c r="H5" s="11">
-        <v>1</v>
+      <c r="H5" s="6">
+        <f>H$2</f>
+        <v>0.25</v>
       </c>
       <c r="I5">
-        <f>($E5-H5)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0.2</v>
+        <f t="shared" ref="I5:I14" si="1">($E5-H5)^2</f>
+        <v>0.5625</v>
+      </c>
+      <c r="J5" s="6">
+        <f>J$2</f>
+        <v>0.15</v>
       </c>
       <c r="K5">
-        <f>($E5-J5)^2</f>
-        <v>0.64000000000000012</v>
+        <f t="shared" ref="K5:K14" si="2">($E5-J5)^2</f>
+        <v>0.72249999999999992</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.3">
@@ -4554,26 +4787,29 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="6">
+        <f t="shared" ref="F6:J14" si="3">F$2</f>
         <v>0.2</v>
       </c>
       <c r="G6">
-        <f>($E6-F6)^2</f>
+        <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
       </c>
-      <c r="H6" s="11">
-        <v>1</v>
+      <c r="H6" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I6">
-        <f>($E6-H6)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0.3</v>
+        <f t="shared" si="1"/>
+        <v>0.5625</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K6">
-        <f>($E6-J6)^2</f>
-        <v>0.48999999999999994</v>
+        <f t="shared" si="2"/>
+        <v>0.72249999999999992</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.3">
@@ -4583,26 +4819,29 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G7">
-        <f>($E7-F7)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H7" s="11">
-        <v>0</v>
+      <c r="H7" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I7">
-        <f>($E7-H7)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K7">
-        <f>($E7-J7)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.3">
@@ -4612,26 +4851,29 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G8">
-        <f>($E8-F8)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H8" s="11">
-        <v>0</v>
+      <c r="H8" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I8">
-        <f>($E8-H8)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K8">
-        <f>($E8-J8)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.3">
@@ -4641,26 +4883,29 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G9">
-        <f>($E9-F9)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H9" s="11">
-        <v>0</v>
+      <c r="H9" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I9">
-        <f>($E9-H9)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K9">
-        <f>($E9-J9)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.3">
@@ -4670,26 +4915,29 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G10">
-        <f>($E10-F10)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H10" s="11">
-        <v>0</v>
+      <c r="H10" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I10">
-        <f>($E10-H10)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K10">
-        <f>($E10-J10)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.3">
@@ -4699,26 +4947,29 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G11">
-        <f>($E11-F11)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H11" s="11">
-        <v>0</v>
+      <c r="H11" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I11">
-        <f>($E11-H11)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K11">
-        <f>($E11-J11)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.3">
@@ -4728,26 +4979,29 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G12">
-        <f>($E12-F12)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H12" s="11">
-        <v>0</v>
+      <c r="H12" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I12">
-        <f>($E12-H12)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K12">
-        <f>($E12-J12)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.3">
@@ -4757,26 +5011,29 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G13">
-        <f>($E13-F13)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H13" s="11">
-        <v>0</v>
+      <c r="H13" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I13">
-        <f>($E13-H13)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K13">
-        <f>($E13-J13)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.3">
@@ -4786,31 +5043,34 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="6">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="G14">
-        <f>($E14-F14)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="H14" s="11">
-        <v>0</v>
+      <c r="H14" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="I14">
-        <f>($E14-H14)^2</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="11">
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="K14">
-        <f>($E14-J14)^2</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="E15" s="10" t="s">
-        <v>136</v>
+      <c r="E15" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="G15" s="8">
         <f>AVERAGE(G5:G14)</f>
@@ -4819,17 +5079,17 @@
       <c r="H15" s="9"/>
       <c r="I15" s="8">
         <f>AVERAGE(I5:I14)</f>
-        <v>0</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="8">
         <f>AVERAGE(K5:K14)</f>
-        <v>0.14500000000000005</v>
+        <v>0.16249999999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4848,7 +5108,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -4874,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5">
         <v>0.11254699999999999</v>
@@ -4903,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>0.114786</v>
@@ -4932,7 +5192,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7">
         <v>0.115136</v>
@@ -4961,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8">
         <v>0.11614099999999999</v>
@@ -4990,7 +5250,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E9">
         <v>0.17508799999999999</v>
@@ -5019,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10">
         <v>0.18465599999999999</v>

</xml_diff>

<commit_message>
Updated spreadsheet with latest presentation times
</commit_message>
<xml_diff>
--- a/SupportingMaterial/Opioid_Support.xlsx
+++ b/SupportingMaterial/Opioid_Support.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camke\OneDrive\Education\Berkeley\W210_Capstone\Project\OpiGit\SupportingMaterial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/615d2bc5d955ad7e/Education/Berkeley/W210_Capstone/Project/OpiGit/SupportingMaterial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="623" documentId="11_F25DC773A252ABDACC1048B4211D4B9E5ADE58E8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2BDFC200-17EC-43E6-9689-E9A359BFCA00}"/>
+  <xr:revisionPtr revIDLastSave="676" documentId="11_F25DC773A252ABDACC1048B4211D4B9E5ADE58E8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FC8DBEC1-564D-432A-9DA3-7696B8901951}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
   <si>
     <t>Model</t>
   </si>
@@ -500,6 +500,19 @@
   </si>
   <si>
     <t>Speed up!</t>
+  </si>
+  <si>
+    <t>PFI callout in wrong place</t>
+  </si>
+  <si>
+    <t>Wed.
+Dry 
+Run #1</t>
+  </si>
+  <si>
+    <t>Wed.
+Dry 
+Run #2</t>
   </si>
 </sst>
 </file>
@@ -666,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,6 +734,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3843,10 +3863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A51846-7BEA-4E25-AD95-1A0EDC9F577F}">
-  <dimension ref="B2:M22"/>
+  <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3854,14 +3874,14 @@
     <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" customWidth="1"/>
-    <col min="5" max="8" width="7.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
-    <col min="10" max="11" width="7.5546875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="7.5546875" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
     <col min="13" max="14" width="7.5546875" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
       <c r="D2" s="10" t="s">
@@ -3872,12 +3892,15 @@
       <c r="G2" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="2:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="30" t="s">
         <v>14</v>
       </c>
@@ -3896,12 +3919,21 @@
       <c r="G3" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="M3" s="3" t="s">
+      <c r="H3" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="37"/>
+      <c r="P3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="32" t="s">
         <v>16</v>
       </c>
@@ -3920,12 +3952,25 @@
       <c r="G4" s="13">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="H4" s="27"/>
-      <c r="M4" t="s">
+      <c r="H4" s="14">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="I4" s="14">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="J4" s="15">
+        <v>9.0972222222222218E-2</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="M4" s="14">
+        <f>STDEV(D4:J4)</f>
+        <v>1.0598067761173738E-2</v>
+      </c>
+      <c r="P4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="32" t="s">
         <v>26</v>
       </c>
@@ -3944,12 +3989,25 @@
       <c r="G5" s="13">
         <v>4.8611111111111112E-2</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="M5" t="s">
+      <c r="H5" s="14">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="I5" s="14">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="J5" s="15">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="M5" s="38">
+        <f>STDEV(D5:J5)</f>
+        <v>1.8744487725884133E-3</v>
+      </c>
+      <c r="P5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
         <v>18</v>
       </c>
@@ -3968,15 +4026,28 @@
       <c r="G6" s="13">
         <v>0.13125000000000001</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" t="s">
+      <c r="H6" s="14">
+        <v>0.13472222222222222</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0.13749999999999998</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" t="s">
         <v>149</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="14">
+        <f>STDEV(D6:H6)</f>
+        <v>1.349618430300731E-2</v>
+      </c>
+      <c r="P6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="32" t="s">
         <v>25</v>
       </c>
@@ -3995,9 +4066,25 @@
       <c r="G7" s="13">
         <v>7.7083333333333337E-2</v>
       </c>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H7" s="14">
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="I7" s="14">
+        <v>7.3611111111111113E-2</v>
+      </c>
+      <c r="J7" s="15">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="14">
+        <f>STDEV(D7:H7)</f>
+        <v>1.2360330811826102E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="32" t="s">
         <v>20</v>
       </c>
@@ -4016,12 +4103,25 @@
       <c r="G8" s="13">
         <v>0.17916666666666667</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="M8" s="3" t="s">
+      <c r="H8" s="14">
+        <v>0.17500000000000002</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0.17847222222222223</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="M8" s="38">
+        <f>STDEV(D8:I8)</f>
+        <v>8.4072722904789537E-3</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
@@ -4040,12 +4140,25 @@
       <c r="G9" s="22">
         <v>7.5694444444444439E-2</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="M9" t="s">
+      <c r="H9" s="23">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I9" s="23">
+        <v>6.805555555555555E-2</v>
+      </c>
+      <c r="J9" s="24">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="M9" s="38">
+        <f>STDEV(D9:J9)</f>
+        <v>4.3632000523969681E-3</v>
+      </c>
+      <c r="P9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="34" t="s">
         <v>24</v>
       </c>
@@ -4066,80 +4179,92 @@
         <f>SUM(G4:G9)</f>
         <v>0.58472222222222214</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="M10" t="s">
+      <c r="H10" s="17">
+        <f>SUM(H4:H9)</f>
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="I10" s="17">
+        <f>SUM(I4:I9)</f>
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="J10" s="18">
+        <f>SUM(J4:J9)</f>
+        <v>0.6</v>
+      </c>
+      <c r="K10" s="38"/>
+      <c r="P10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M11" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>147</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M13" t="s">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M14" t="s">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M15" t="s">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M16" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L17" t="s">
+    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L18" t="s">
+    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L19" t="s">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
         <v>21</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="M20" t="s">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="P20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="M21" t="s">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="P21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="M22" t="s">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated spreadsheet times for dry run
</commit_message>
<xml_diff>
--- a/SupportingMaterial/Opioid_Support.xlsx
+++ b/SupportingMaterial/Opioid_Support.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/615d2bc5d955ad7e/Education/Berkeley/W210_Capstone/Project/OpiGit/SupportingMaterial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="676" documentId="11_F25DC773A252ABDACC1048B4211D4B9E5ADE58E8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FC8DBEC1-564D-432A-9DA3-7696B8901951}"/>
+  <xr:revisionPtr revIDLastSave="707" documentId="11_F25DC773A252ABDACC1048B4211D4B9E5ADE58E8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3C176F12-E41C-4781-883B-76727BAE8F3E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Comparison" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="157">
   <si>
     <t>Model</t>
   </si>
@@ -513,6 +513,20 @@
     <t>Wed.
 Dry 
 Run #2</t>
+  </si>
+  <si>
+    <t>Showcase!</t>
+  </si>
+  <si>
+    <t>Thurs.
+Show-
+case</t>
+  </si>
+  <si>
+    <t>Wed. Dry Run</t>
+  </si>
+  <si>
+    <t>Thurs. Dry Run</t>
   </si>
 </sst>
 </file>
@@ -3863,10 +3877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A51846-7BEA-4E25-AD95-1A0EDC9F577F}">
-  <dimension ref="B2:P22"/>
+  <dimension ref="B2:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3874,14 +3888,14 @@
     <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" customWidth="1"/>
-    <col min="5" max="11" width="7.5546875" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
-    <col min="13" max="14" width="7.5546875" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="14" width="7.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" customWidth="1"/>
     <col min="16" max="17" width="7.5546875" customWidth="1"/>
+    <col min="18" max="18" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
       <c r="D2" s="10" t="s">
@@ -3895,12 +3909,17 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
       <c r="J2" s="25"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="K2" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="25"/>
       <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="2:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="30" t="s">
         <v>14</v>
       </c>
@@ -3928,12 +3947,21 @@
       <c r="J3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="P3" s="3" t="s">
+      <c r="K3" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="N3" s="37"/>
+      <c r="S3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="32" t="s">
         <v>16</v>
       </c>
@@ -3961,16 +3989,21 @@
       <c r="J4" s="15">
         <v>9.0972222222222218E-2</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="M4" s="14">
-        <f>STDEV(D4:J4)</f>
-        <v>1.0598067761173738E-2</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="K4" s="14">
+        <v>9.375E-2</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="14"/>
+      <c r="P4" s="14">
+        <f>STDEV(D4:M4)</f>
+        <v>1.1234434656263594E-2</v>
+      </c>
+      <c r="S4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="32" t="s">
         <v>26</v>
       </c>
@@ -3998,16 +4031,21 @@
       <c r="J5" s="15">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="M5" s="38">
-        <f>STDEV(D5:J5)</f>
-        <v>1.8744487725884133E-3</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="K5" s="14">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="14"/>
+      <c r="P5" s="38">
+        <f>STDEV(D5:M5)</f>
+        <v>1.8349822731243987E-3</v>
+      </c>
+      <c r="S5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
         <v>18</v>
       </c>
@@ -4035,19 +4073,24 @@
       <c r="J6" s="15">
         <v>0.13749999999999998</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" t="s">
+      <c r="K6" s="14">
+        <v>0.13263888888888889</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="14"/>
+      <c r="O6" t="s">
         <v>149</v>
       </c>
-      <c r="M6" s="14">
+      <c r="P6" s="14">
         <f>STDEV(D6:H6)</f>
         <v>1.349618430300731E-2</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="32" t="s">
         <v>25</v>
       </c>
@@ -4075,16 +4118,21 @@
       <c r="J7" s="15">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" t="s">
+      <c r="K7" s="14">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="14"/>
+      <c r="O7" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="14">
+      <c r="P7" s="14">
         <f>STDEV(D7:H7)</f>
         <v>1.2360330811826102E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="32" t="s">
         <v>20</v>
       </c>
@@ -4112,16 +4160,21 @@
       <c r="J8" s="15">
         <v>0.17847222222222223</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="M8" s="38">
+      <c r="K8" s="14">
+        <v>0.18472222222222223</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="14"/>
+      <c r="P8" s="38">
         <f>STDEV(D8:I8)</f>
         <v>8.4072722904789537E-3</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
@@ -4149,122 +4202,139 @@
       <c r="J9" s="24">
         <v>7.0833333333333331E-2</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="M9" s="38">
-        <f>STDEV(D9:J9)</f>
-        <v>4.3632000523969681E-3</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="K9" s="23">
+        <v>7.2222222222222229E-2</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="14"/>
+      <c r="P9" s="38">
+        <f>STDEV(D9:M9)</f>
+        <v>4.0651912466861907E-3</v>
+      </c>
+      <c r="S9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="34" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="16">
-        <f>SUM(D4:D9)</f>
+        <f t="shared" ref="D10:M10" si="0">SUM(D4:D9)</f>
         <v>0.57847222222222217</v>
       </c>
       <c r="E10" s="17">
-        <f>SUM(E4:E9)</f>
+        <f t="shared" si="0"/>
         <v>0.53819444444444442</v>
       </c>
       <c r="F10" s="18">
-        <f>SUM(F4:F9)</f>
+        <f t="shared" si="0"/>
         <v>0.56597222222222221</v>
       </c>
       <c r="G10" s="16">
-        <f>SUM(G4:G9)</f>
+        <f t="shared" si="0"/>
         <v>0.58472222222222214</v>
       </c>
       <c r="H10" s="17">
-        <f>SUM(H4:H9)</f>
+        <f t="shared" si="0"/>
         <v>0.59305555555555556</v>
       </c>
       <c r="I10" s="17">
-        <f>SUM(I4:I9)</f>
+        <f t="shared" si="0"/>
         <v>0.58680555555555558</v>
       </c>
       <c r="J10" s="18">
-        <f>SUM(J4:J9)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="P10" t="s">
+      <c r="K10" s="16">
+        <f t="shared" si="0"/>
+        <v>0.60694444444444451</v>
+      </c>
+      <c r="L10" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="38"/>
+      <c r="S10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P11" t="s">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>147</v>
       </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P13" t="s">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P14" t="s">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P15" t="s">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P16" t="s">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O17" t="s">
+    <row r="17" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R17" t="s">
         <v>21</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O18" t="s">
+    <row r="18" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O19" t="s">
+    <row r="19" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R19" t="s">
         <v>21</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="P20" t="s">
+    <row r="20" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="P21" t="s">
+    <row r="21" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="S21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="P22" t="s">
+    <row r="22" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="S22" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>